<commit_message>
Rename panic_high to maxpanic and panic_low to minpanic
</commit_message>
<xml_diff>
--- a/bhp/lims/resources/results_ranges.xlsx
+++ b/bhp/lims/resources/results_ranges.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1691" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1691" uniqueCount="130">
   <si>
     <t>keyword</t>
   </si>
@@ -44,10 +44,10 @@
     <t>age_to</t>
   </si>
   <si>
-    <t>panic_high</t>
-  </si>
-  <si>
-    <t>panic_low</t>
+    <t>maxpanic</t>
+  </si>
+  <si>
+    <t>minpanic</t>
   </si>
   <si>
     <t>ALB</t>
@@ -408,9 +408,6 @@
   </si>
   <si>
     <t>366d</t>
-  </si>
-  <si>
-    <t> MONO1</t>
   </si>
 </sst>
 </file>
@@ -571,7 +568,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="TableStyleLight1" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in TableStyleLight1" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -583,8 +580,8 @@
   </sheetPr>
   <dimension ref="A1:J335"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A157" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A253" activeCellId="0" sqref="A253"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -7037,7 +7034,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="242" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="9" t="s">
         <v>97</v>
       </c>
@@ -7951,7 +7948,7 @@
     </row>
     <row r="280" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="9" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="B280" s="9" t="s">
         <v>53</v>
@@ -7975,7 +7972,7 @@
     </row>
     <row r="281" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="9" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="B281" s="9" t="s">
         <v>53</v>
@@ -7999,7 +7996,7 @@
     </row>
     <row r="282" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="9" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="B282" s="9" t="s">
         <v>53</v>
@@ -8023,7 +8020,7 @@
     </row>
     <row r="283" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="9" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="B283" s="9" t="s">
         <v>53</v>
@@ -8047,7 +8044,7 @@
     </row>
     <row r="284" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="9" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="B284" s="9" t="s">
         <v>53</v>
@@ -8071,7 +8068,7 @@
     </row>
     <row r="285" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="9" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="B285" s="9" t="s">
         <v>53</v>
@@ -8095,7 +8092,7 @@
     </row>
     <row r="286" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="9" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="B286" s="9" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Enable critical result alert for RNA PCR result >39 copies per ml (#241)
* Remove get_next_id from ng view

This function has been removed from senaite.core:
https://github.com/senaite/senaite.core/pull/1364

* Fallback to Panic level range if no grading defined

If an analysis service does not have any grading defined, fallback
to the "classic" panic level range when checking if the result
for an analysis must be considered in a threatening condition

* Set max_panic for HIV Viral Load (RNA PCR) AUVL to 40 copies/ml
</commit_message>
<xml_diff>
--- a/bhp/lims/resources/results_ranges.xlsx
+++ b/bhp/lims/resources/results_ranges.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="621" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="572" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis Specifications" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,13 +16,14 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Analysis Specifications'!$A$340:$A$349</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Analysis Specifications'!$A$340:$A$349</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Analysis Specifications'!$A$340:$A$349</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Analysis Specifications'!$A$340:$A$349</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1784" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1789" uniqueCount="154">
   <si>
     <t>keyword</t>
   </si>
@@ -482,6 +483,9 @@
   <si>
     <t>BILTS</t>
   </si>
+  <si>
+    <t>AUVL</t>
+  </si>
 </sst>
 </file>
 
@@ -655,7 +659,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in TableStyleLight1" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -669,10 +673,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z349"/>
+  <dimension ref="A1:Z350"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A316" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B348" activeCellId="0" sqref="B348"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A310" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C351" activeCellId="0" sqref="C351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -683,20 +687,7 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.8265306122449"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="15"/>
     <col collapsed="false" hidden="false" max="10" min="6" style="2" width="8.8265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="13.6632653061225"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="3" width="12.8316326530612"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="3" width="14.5"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="3" width="15.1632653061224"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="3" width="11.8367346938776"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="12.5"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="3" width="14.6581632653061"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="3" width="18.8367346938776"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="3" width="20.6632653061224"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="3" width="19.6632653061224"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="3" width="20.1683673469388"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="3" width="21.1683673469388"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="3" width="16"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="3" width="19.3316326530612"/>
+    <col collapsed="false" hidden="false" max="26" min="11" style="3" width="8.6734693877551"/>
     <col collapsed="false" hidden="false" max="1025" min="27" style="3" width="8.8265306122449"/>
   </cols>
   <sheetData>
@@ -17174,7 +17165,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="348" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="8" t="s">
         <v>152</v>
       </c>
@@ -17224,6 +17215,32 @@
       </c>
       <c r="I349" s="2" t="n">
         <v>75</v>
+      </c>
+    </row>
+    <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A350" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B350" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C350" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D350" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="F350" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G350" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H350" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I350" s="2" t="n">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>